<commit_message>
Add skeleton regex builder GUI, add new funcs - Added RegexEscape to get the same functionality as re.escape in Python - Added RegexFindObject to make it easy to find a single match object for a regex that matches in multiple places - Added a simple GUI which I will eventually make work so that it can be used to design regular expressions.
</commit_message>
<xml_diff>
--- a/regexfunctions_addin_test.xlsx
+++ b/regexfunctions_addin_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjols\Documents\Macros VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD52BBD-9267-45BF-849E-5838CFF937E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB5E04-81B6-43E8-BCEF-7F0EA2DD08A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7E2FE77-3AC4-47C5-AD0A-77BDB3E74EA4}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>strings</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Dab</t>
+  </si>
+  <si>
+    <t>RegexEscape on the_regex</t>
   </si>
 </sst>
 </file>
@@ -210,12 +213,13 @@
     </sheetNames>
     <definedNames>
       <definedName name="Regexcontains"/>
+      <definedName name="regexescape"/>
       <definedName name="regexfind"/>
       <definedName name="Regexfindall"/>
       <definedName name="regexfullmatch"/>
       <definedName name="regexmatch"/>
       <definedName name="regexmatchend"/>
-      <definedName name="RegexReplace"/>
+      <definedName name="regexreplacE"/>
       <definedName name="RegexSplitToString"/>
     </definedNames>
     <sheetDataSet>
@@ -525,23 +529,23 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -594,19 +598,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2">[1]!RegexReplace($A$9, "$2$1", A2)</f>
+        <f t="array" ref="B2">[1]!regexreplacE($A$9, "$2$1", A2)</f>
         <v>a big bad dawg</v>
       </c>
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2" xml:space="preserve"> [1]!RegexReplace($A$9, "$2$1", A2, TRUE, TRUE)</f>
+        <f t="array" ref="C2" xml:space="preserve"> [1]!regexreplacE($A$9, "$2$1", A2, TRUE, TRUE)</f>
         <v>a big bda adwg</v>
       </c>
       <c r="D2" t="str" cm="1">
-        <f t="array" ref="D2">[1]!RegexReplace($A$9,"$2$1", A2, FALSE, FALSE)</f>
+        <f t="array" ref="D2">[1]!regexreplacE($A$9,"$2$1", A2, FALSE, FALSE)</f>
         <v>a big bad dawg</v>
       </c>
       <c r="E2" t="str" cm="1">
-        <f t="array" ref="E2">[1]!RegexReplace($A$9, "$2$1", A2, FALSE, TRUE)</f>
+        <f t="array" ref="E2">[1]!regexreplacE($A$9, "$2$1", A2, FALSE, TRUE)</f>
         <v>a big bda dawg</v>
       </c>
       <c r="F2" t="b" cm="1">
@@ -651,19 +655,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">[1]!RegexReplace($A$9, "$2$1", A3)</f>
+        <f t="array" ref="B3">[1]!regexreplacE($A$9, "$2$1", A3)</f>
         <v>a big bad aDwg</v>
       </c>
       <c r="C3" t="str" cm="1">
-        <f t="array" ref="C3" xml:space="preserve"> [1]!RegexReplace($A$9, "$2$1", A3, TRUE, TRUE)</f>
+        <f t="array" ref="C3" xml:space="preserve"> [1]!regexreplacE($A$9, "$2$1", A3, TRUE, TRUE)</f>
         <v>a big bda aDwg</v>
       </c>
       <c r="D3" t="str" cm="1">
-        <f t="array" ref="D3">[1]!RegexReplace($A$9,"$2$1", A3, FALSE, FALSE)</f>
+        <f t="array" ref="D3">[1]!regexreplacE($A$9,"$2$1", A3, FALSE, FALSE)</f>
         <v>a big bad aDwg</v>
       </c>
       <c r="E3" t="str" cm="1">
-        <f t="array" ref="E3">[1]!RegexReplace($A$9, "$2$1", A3, FALSE, TRUE)</f>
+        <f t="array" ref="E3">[1]!regexreplacE($A$9, "$2$1", A3, FALSE, TRUE)</f>
         <v>a big bda Dawg</v>
       </c>
       <c r="F3" t="b" cm="1">
@@ -708,19 +712,19 @@
         <v>15</v>
       </c>
       <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4">[1]!RegexReplace($A$9, "$2$1", A4)</f>
+        <f t="array" ref="B4">[1]!regexreplacE($A$9, "$2$1", A4)</f>
         <v>a big bDa dawg</v>
       </c>
       <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4" xml:space="preserve"> [1]!RegexReplace($A$9, "$2$1", A4, TRUE, TRUE)</f>
+        <f t="array" ref="C4" xml:space="preserve"> [1]!regexreplacE($A$9, "$2$1", A4, TRUE, TRUE)</f>
         <v>a big bDa adwg</v>
       </c>
       <c r="D4" t="str" cm="1">
-        <f t="array" ref="D4">[1]!RegexReplace($A$9,"$2$1", A4, FALSE, FALSE)</f>
+        <f t="array" ref="D4">[1]!regexreplacE($A$9,"$2$1", A4, FALSE, FALSE)</f>
         <v>a big bDa dawg</v>
       </c>
       <c r="E4" t="str" cm="1">
-        <f t="array" ref="E4">[1]!RegexReplace($A$9, "$2$1", A4, FALSE, TRUE)</f>
+        <f t="array" ref="E4">[1]!regexreplacE($A$9, "$2$1", A4, FALSE, TRUE)</f>
         <v>a big bDa dawg</v>
       </c>
       <c r="F4" t="b" cm="1">
@@ -765,19 +769,19 @@
         <v>16</v>
       </c>
       <c r="B5" t="str" cm="1">
-        <f t="array" ref="B5">[1]!RegexReplace($A$9, "$2$1", A5)</f>
+        <f t="array" ref="B5">[1]!regexreplacE($A$9, "$2$1", A5)</f>
         <v>a big bDa aDwg</v>
       </c>
       <c r="C5" t="str" cm="1">
-        <f t="array" ref="C5" xml:space="preserve"> [1]!RegexReplace($A$9, "$2$1", A5, TRUE, TRUE)</f>
+        <f t="array" ref="C5" xml:space="preserve"> [1]!regexreplacE($A$9, "$2$1", A5, TRUE, TRUE)</f>
         <v>a big bDa aDwg</v>
       </c>
       <c r="D5" t="str" cm="1">
-        <f t="array" ref="D5">[1]!RegexReplace($A$9,"$2$1", A5, FALSE, FALSE)</f>
+        <f t="array" ref="D5">[1]!regexreplacE($A$9,"$2$1", A5, FALSE, FALSE)</f>
         <v>a big bDa Dawg</v>
       </c>
       <c r="E5" t="str" cm="1">
-        <f t="array" ref="E5">[1]!RegexReplace($A$9, "$2$1", A5, FALSE, TRUE)</f>
+        <f t="array" ref="E5">[1]!regexreplacE($A$9, "$2$1", A5, FALSE, TRUE)</f>
         <v>a big bDa Dawg</v>
       </c>
       <c r="F5" t="b" cm="1">
@@ -821,10 +825,17 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" t="str" cm="1">
+        <f t="array" ref="C9">[1]!regexescape(A9)</f>
+        <v>\(\[aD\]\)\(\[aD\]\)</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>